<commit_message>
Working on energy data.
</commit_message>
<xml_diff>
--- a/data/energy_ecc.xlsx
+++ b/data/energy_ecc.xlsx
@@ -1160,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="7" t="n">
-        <v>0.000689849763500573</v>
+        <v>0.000689849763500575</v>
       </c>
       <c r="AK6" s="7" t="n">
         <v>0</v>
@@ -1172,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="AN6" s="7" t="n">
-        <v>0.00803046323109937</v>
+        <v>0.00803046323109933</v>
       </c>
       <c r="AO6" s="7" t="n">
         <v>0</v>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
       <c r="AS6" s="7" t="n">
-        <v>0.0009125481540941</v>
+        <v>0.000912548154094104</v>
       </c>
       <c r="AT6" s="7" t="n">
         <v>0</v>
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="AI14" s="7" t="n">
-        <v>0.00541779963957506</v>
+        <v>0.00541779963957512</v>
       </c>
       <c r="AJ14" s="7" t="n">
         <v>0</v>
@@ -1986,7 +1986,7 @@
         <v>0</v>
       </c>
       <c r="AZ14" s="7" t="n">
-        <v>0.72465121788954</v>
+        <v>0.724651217889545</v>
       </c>
       <c r="BA14" s="7" t="n">
         <v>0</v>
@@ -2265,7 +2265,7 @@
         <v>0</v>
       </c>
       <c r="AS17" s="7" t="n">
-        <v>0.00119734058540369</v>
+        <v>0.00119734058540368</v>
       </c>
       <c r="AT17" s="7" t="n">
         <v>0</v>
@@ -2715,7 +2715,7 @@
         <v>0</v>
       </c>
       <c r="AJ25" s="7" t="n">
-        <v>0.00503330546857328</v>
+        <v>0.0050333054685733</v>
       </c>
       <c r="AK25" s="7" t="n">
         <v>0</v>
@@ -2759,7 +2759,7 @@
         <v>5</v>
       </c>
       <c r="AG26" s="7" t="n">
-        <v>-0.0000000000000000174402691487679</v>
+        <v>-0.0000000000000000330796384606328</v>
       </c>
       <c r="AH26" s="7" t="n">
         <v>0</v>
@@ -2821,10 +2821,10 @@
         <v>0</v>
       </c>
       <c r="AJ27" s="7" t="n">
-        <v>0.00740737994440796</v>
+        <v>0.00740737994440806</v>
       </c>
       <c r="AK27" s="7" t="n">
-        <v>-0.0000000000000000249147397265229</v>
+        <v>-0.0000000000000000472567582222416</v>
       </c>
       <c r="AL27" s="7" t="n">
         <v>0</v>
@@ -2898,7 +2898,7 @@
         <v>0</v>
       </c>
       <c r="AR28" s="7" t="n">
-        <v>0.0000791571234708902</v>
+        <v>0.0000791571234708916</v>
       </c>
       <c r="AS28" s="7" t="n">
         <v>0.0250544289288924</v>
@@ -3045,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="AN31" s="7" t="n">
-        <v>0.000282479404278675</v>
+        <v>0.00028247940427868</v>
       </c>
       <c r="AO31" s="7" t="n">
         <v>0</v>
@@ -3098,10 +3098,10 @@
         <v>0</v>
       </c>
       <c r="AN32" s="7" t="n">
-        <v>0.000575922630853108</v>
+        <v>0.000575922630853104</v>
       </c>
       <c r="AO32" s="7" t="n">
-        <v>0.000208570467020405</v>
+        <v>0.000208570467020404</v>
       </c>
       <c r="AP32" s="7" t="n">
         <v>0</v>
@@ -3199,7 +3199,7 @@
         <v>0</v>
       </c>
       <c r="AM34" s="7" t="n">
-        <v>0.00098993535374629</v>
+        <v>0.00098993535374628</v>
       </c>
       <c r="AN34" s="7" t="n">
         <v>0</v>
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="AP34" s="7" t="n">
-        <v>26.2904528311585</v>
+        <v>26.2904528311586</v>
       </c>
       <c r="AQ34" s="7" t="n">
         <v>0</v>
@@ -3261,10 +3261,10 @@
         <v>0</v>
       </c>
       <c r="AR35" s="7" t="n">
-        <v>0.000185976854428328</v>
+        <v>0.00018597685442833</v>
       </c>
       <c r="AS35" s="7" t="n">
-        <v>0.000185976854428328</v>
+        <v>0.00018597685442833</v>
       </c>
       <c r="AT35" s="7" t="n">
         <v>0</v>
@@ -3299,13 +3299,13 @@
         <v>0</v>
       </c>
       <c r="AO36" s="7" t="n">
-        <v>0.0079744540502882</v>
+        <v>0.0079744540502881</v>
       </c>
       <c r="AP36" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AQ36" s="7" t="n">
-        <v>0.0220197452777908</v>
+        <v>0.0220197452777906</v>
       </c>
       <c r="AR36" s="7" t="n">
         <v>0</v>
@@ -3328,22 +3328,22 @@
         <v>0</v>
       </c>
       <c r="AI37" s="7" t="n">
-        <v>0.00205862419830071</v>
+        <v>0.00205862419830068</v>
       </c>
       <c r="AJ37" s="7" t="n">
-        <v>0.345567475615063</v>
+        <v>0.345567475615068</v>
       </c>
       <c r="AK37" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AL37" s="7" t="n">
-        <v>0.0000000000000000105647885717917</v>
+        <v>-0.0000000000000000127789214296028</v>
       </c>
       <c r="AM37" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AN37" s="7" t="n">
-        <v>0.360438320942659</v>
+        <v>0.360438320942663</v>
       </c>
       <c r="AO37" s="7" t="n">
         <v>0</v>
@@ -3408,7 +3408,7 @@
         <v>0</v>
       </c>
       <c r="AT38" s="7" t="n">
-        <v>0.00202357682087733</v>
+        <v>0.00202357682087738</v>
       </c>
     </row>
     <row r="39">
@@ -3419,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="AH39" s="7" t="n">
-        <v>-0.00000000000000000153448598829721</v>
+        <v>-0.000000000000000000485138520369623</v>
       </c>
       <c r="AI39" s="7" t="n">
         <v>0</v>
@@ -3437,10 +3437,10 @@
         <v>0</v>
       </c>
       <c r="AN39" s="7" t="n">
-        <v>0.000523435943068145</v>
+        <v>0.000523435943068142</v>
       </c>
       <c r="AO39" s="7" t="n">
-        <v>0.0147104781502635</v>
+        <v>0.0147104781502632</v>
       </c>
       <c r="AP39" s="7" t="n">
         <v>0</v>
@@ -3531,10 +3531,10 @@
         <v>0</v>
       </c>
       <c r="AN41" s="7" t="n">
-        <v>0.00000978759390537482</v>
+        <v>0.00000978759390537483</v>
       </c>
       <c r="AO41" s="7" t="n">
-        <v>0.00000354457859873677</v>
+        <v>0.00000354457859873676</v>
       </c>
       <c r="AP41" s="7" t="n">
         <v>0</v>
@@ -3625,10 +3625,10 @@
         <v>0</v>
       </c>
       <c r="AN43" s="7" t="n">
-        <v>0.00000515136521335517</v>
+        <v>0.00000515136521335513</v>
       </c>
       <c r="AO43" s="7" t="n">
-        <v>0.00000186556768354567</v>
+        <v>0.00000186556768354565</v>
       </c>
       <c r="AP43" s="7" t="n">
         <v>0</v>
@@ -3719,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="AJ48" s="6" t="n">
-        <v>0.00503330546857328</v>
+        <v>0.0050333054685733</v>
       </c>
       <c r="AK48" s="6" t="n">
         <v>0</v>
@@ -3763,7 +3763,7 @@
         <v>5</v>
       </c>
       <c r="AG49" s="6" t="n">
-        <v>-0.0000000000000000174402691487679</v>
+        <v>-0.0000000000000000330796384606328</v>
       </c>
       <c r="AH49" s="6" t="n">
         <v>0</v>
@@ -3825,10 +3825,10 @@
         <v>0</v>
       </c>
       <c r="AJ50" s="6" t="n">
-        <v>0.00740737994440796</v>
+        <v>0.00740737994440806</v>
       </c>
       <c r="AK50" s="6" t="n">
-        <v>-0.0000000000000000249147397265229</v>
+        <v>-0.0000000000000000472567582222416</v>
       </c>
       <c r="AL50" s="6" t="n">
         <v>0</v>
@@ -3902,7 +3902,7 @@
         <v>0</v>
       </c>
       <c r="AR51" s="6" t="n">
-        <v>0.0000791571234708902</v>
+        <v>0.0000791571234708916</v>
       </c>
       <c r="AS51" s="6" t="n">
         <v>0.0250544289288924</v>
@@ -3931,7 +3931,7 @@
         <v>0</v>
       </c>
       <c r="AJ52" s="6" t="n">
-        <v>0.000689849763500573</v>
+        <v>0.000689849763500575</v>
       </c>
       <c r="AK52" s="6" t="n">
         <v>0</v>
@@ -3943,7 +3943,7 @@
         <v>0</v>
       </c>
       <c r="AN52" s="6" t="n">
-        <v>0.00803046323109937</v>
+        <v>0.00803046323109933</v>
       </c>
       <c r="AO52" s="6" t="n">
         <v>0</v>
@@ -3958,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="AS52" s="6" t="n">
-        <v>0.0009125481540941</v>
+        <v>0.000912548154094104</v>
       </c>
       <c r="AT52" s="6" t="n">
         <v>0</v>
@@ -4049,7 +4049,7 @@
         <v>0</v>
       </c>
       <c r="AN54" s="6" t="n">
-        <v>0.000282479404278675</v>
+        <v>0.00028247940427868</v>
       </c>
       <c r="AO54" s="6" t="n">
         <v>0</v>
@@ -4102,10 +4102,10 @@
         <v>0</v>
       </c>
       <c r="AN55" s="6" t="n">
-        <v>0.000575922630853108</v>
+        <v>0.000575922630853104</v>
       </c>
       <c r="AO55" s="6" t="n">
-        <v>0.000208570467020405</v>
+        <v>0.000208570467020404</v>
       </c>
       <c r="AP55" s="6" t="n">
         <v>0</v>
@@ -4205,7 +4205,7 @@
         <v>0</v>
       </c>
       <c r="AM57" s="6" t="n">
-        <v>0.00098993535374629</v>
+        <v>0.00098993535374628</v>
       </c>
       <c r="AN57" s="6" t="n">
         <v>0</v>
@@ -4214,7 +4214,7 @@
         <v>0</v>
       </c>
       <c r="AP57" s="6" t="n">
-        <v>26.2904528311585</v>
+        <v>26.2904528311586</v>
       </c>
       <c r="AQ57" s="6" t="n">
         <v>0</v>
@@ -4273,10 +4273,10 @@
         <v>0</v>
       </c>
       <c r="AR58" s="6" t="n">
-        <v>0.000185976854428328</v>
+        <v>0.00018597685442833</v>
       </c>
       <c r="AS58" s="6" t="n">
-        <v>0.000185976854428328</v>
+        <v>0.00018597685442833</v>
       </c>
       <c r="AT58" s="6" t="n">
         <v>0</v>
@@ -4317,13 +4317,13 @@
         <v>0</v>
       </c>
       <c r="AO59" s="6" t="n">
-        <v>0.0079744540502882</v>
+        <v>0.0079744540502881</v>
       </c>
       <c r="AP59" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AQ59" s="6" t="n">
-        <v>0.0220197452777908</v>
+        <v>0.0220197452777906</v>
       </c>
       <c r="AR59" s="6" t="n">
         <v>0</v>
@@ -4352,22 +4352,22 @@
         <v>0</v>
       </c>
       <c r="AI60" s="6" t="n">
-        <v>0.00747642383787577</v>
+        <v>0.0074764238378758</v>
       </c>
       <c r="AJ60" s="6" t="n">
-        <v>0.345567475615063</v>
+        <v>0.345567475615068</v>
       </c>
       <c r="AK60" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL60" s="6" t="n">
-        <v>0.0000000000000000105647885717917</v>
+        <v>-0.0000000000000000127789214296028</v>
       </c>
       <c r="AM60" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AN60" s="6" t="n">
-        <v>0.360438320942659</v>
+        <v>0.360438320942663</v>
       </c>
       <c r="AO60" s="6" t="n">
         <v>0</v>
@@ -4438,7 +4438,7 @@
         <v>0</v>
       </c>
       <c r="AT61" s="6" t="n">
-        <v>0.00202357682087733</v>
+        <v>0.00202357682087738</v>
       </c>
       <c r="AW61" s="4" t="s">
         <v>21</v>
@@ -4455,7 +4455,7 @@
         <v>0</v>
       </c>
       <c r="AH62" s="6" t="n">
-        <v>-0.00000000000000000153448598829721</v>
+        <v>-0.000000000000000000485138520369623</v>
       </c>
       <c r="AI62" s="6" t="n">
         <v>0</v>
@@ -4473,10 +4473,10 @@
         <v>0</v>
       </c>
       <c r="AN62" s="6" t="n">
-        <v>0.000523435943068145</v>
+        <v>0.000523435943068142</v>
       </c>
       <c r="AO62" s="6" t="n">
-        <v>0.0147104781502635</v>
+        <v>0.0147104781502632</v>
       </c>
       <c r="AP62" s="6" t="n">
         <v>0</v>
@@ -4541,7 +4541,7 @@
         <v>0</v>
       </c>
       <c r="AS63" s="6" t="n">
-        <v>0.00119734058540369</v>
+        <v>0.00119734058540368</v>
       </c>
       <c r="AT63" s="6" t="n">
         <v>0</v>
@@ -4579,10 +4579,10 @@
         <v>0</v>
       </c>
       <c r="AN64" s="6" t="n">
-        <v>0.00000978759390537482</v>
+        <v>0.00000978759390537483</v>
       </c>
       <c r="AO64" s="6" t="n">
-        <v>0.00000354457859873677</v>
+        <v>0.00000354457859873676</v>
       </c>
       <c r="AP64" s="6" t="n">
         <v>0</v>
@@ -4685,10 +4685,10 @@
         <v>0</v>
       </c>
       <c r="AN66" s="6" t="n">
-        <v>0.00000515136521335517</v>
+        <v>0.00000515136521335513</v>
       </c>
       <c r="AO66" s="6" t="n">
-        <v>0.00000186556768354567</v>
+        <v>0.00000186556768354565</v>
       </c>
       <c r="AP66" s="6" t="n">
         <v>0</v>
@@ -4822,7 +4822,7 @@
         <v>0</v>
       </c>
       <c r="D71" s="6" t="n">
-        <v>-0.00000000000000000697609935074109</v>
+        <v>-0.0000000000000000132318396246926</v>
       </c>
       <c r="E71" s="6" t="n">
         <v>0</v>
@@ -4914,7 +4914,7 @@
         <v>0</v>
       </c>
       <c r="E72" s="6" t="n">
-        <v>-0.000000000000000000230172103231791</v>
+        <v>-0.000000000000000000072770526706567</v>
       </c>
       <c r="F72" s="6" t="n">
         <v>0</v>
@@ -5054,7 +5054,7 @@
         <v>0</v>
       </c>
       <c r="V73" s="6" t="n">
-        <v>0.00149598286421847</v>
+        <v>0.00149598286421846</v>
       </c>
       <c r="W73" s="6" t="n">
         <v>0</v>
@@ -5083,7 +5083,7 @@
         <v>37</v>
       </c>
       <c r="B74" s="6" t="n">
-        <v>0.00252907541244832</v>
+        <v>0.00252907541244834</v>
       </c>
       <c r="C74" s="6" t="n">
         <v>0</v>
@@ -5101,7 +5101,7 @@
         <v>0</v>
       </c>
       <c r="H74" s="6" t="n">
-        <v>0.00334311470413482</v>
+        <v>0.00334311470413485</v>
       </c>
       <c r="I74" s="6" t="n">
         <v>0</v>
@@ -5140,7 +5140,7 @@
         <v>0</v>
       </c>
       <c r="U74" s="6" t="n">
-        <v>0.352135970911461</v>
+        <v>0.352135970911465</v>
       </c>
       <c r="V74" s="6" t="n">
         <v>0</v>
@@ -5184,7 +5184,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="6" t="n">
-        <v>-0.0000000000000000174402666556886</v>
+        <v>-0.0000000000000000330796337319121</v>
       </c>
       <c r="G75" s="6" t="n">
         <v>0</v>
@@ -5291,7 +5291,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="6" t="n">
-        <v>0.00000000000000000284177220631046</v>
+        <v>-0.00000000000000000343734126797693</v>
       </c>
       <c r="M76" s="6" t="n">
         <v>0</v>
@@ -5410,7 +5410,7 @@
         <v>0</v>
       </c>
       <c r="V77" s="6" t="n">
-        <v>0.000527593956658866</v>
+        <v>0.000527593956658863</v>
       </c>
       <c r="W77" s="6" t="n">
         <v>0</v>
@@ -5564,7 +5564,7 @@
         <v>0</v>
       </c>
       <c r="N79" s="6" t="n">
-        <v>0.000392246548936757</v>
+        <v>0.000392246548936754</v>
       </c>
       <c r="O79" s="6" t="n">
         <v>0</v>
@@ -5582,7 +5582,7 @@
         <v>0</v>
       </c>
       <c r="T79" s="6" t="n">
-        <v>0.0149970996640395</v>
+        <v>0.0149970996640393</v>
       </c>
       <c r="U79" s="6" t="n">
         <v>0</v>
@@ -5597,19 +5597,19 @@
         <v>0</v>
       </c>
       <c r="Y79" s="6" t="n">
-        <v>0.00759807742213925</v>
+        <v>0.00759807742213906</v>
       </c>
       <c r="Z79" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AA79" s="6" t="n">
-        <v>0.00000666608625205579</v>
+        <v>0.0000066660862520558</v>
       </c>
       <c r="AB79" s="6" t="n">
-        <v>0.0000986853739616356</v>
+        <v>0.0000986853739616354</v>
       </c>
       <c r="AC79" s="6" t="n">
-        <v>0.00000350846644845042</v>
+        <v>0.00000350846644845039</v>
       </c>
     </row>
     <row r="80">
@@ -5665,7 +5665,7 @@
         <v>0</v>
       </c>
       <c r="R80" s="6" t="n">
-        <v>26.2904528311585</v>
+        <v>26.2904528311586</v>
       </c>
       <c r="S80" s="6" t="n">
         <v>0</v>
@@ -5730,7 +5730,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="6" t="n">
-        <v>0.00726651594167098</v>
+        <v>0.00726651594167101</v>
       </c>
       <c r="K81" s="6" t="n">
         <v>0</v>
@@ -5816,7 +5816,7 @@
         <v>0</v>
       </c>
       <c r="I82" s="6" t="n">
-        <v>0.0000791571234708903</v>
+        <v>0.0000791571234708916</v>
       </c>
       <c r="J82" s="6" t="n">
         <v>0</v>
@@ -5846,7 +5846,7 @@
         <v>0</v>
       </c>
       <c r="S82" s="6" t="n">
-        <v>0.000185976854428328</v>
+        <v>0.00018597685442833</v>
       </c>
       <c r="T82" s="6" t="n">
         <v>0</v>
@@ -5917,7 +5917,7 @@
         <v>0</v>
       </c>
       <c r="M83" s="6" t="n">
-        <v>0.00562178964295917</v>
+        <v>0.00562178964295918</v>
       </c>
       <c r="N83" s="6" t="n">
         <v>0</v>
@@ -5956,7 +5956,7 @@
         <v>0</v>
       </c>
       <c r="Z83" s="6" t="n">
-        <v>0.00119734058540369</v>
+        <v>0.00119734058540368</v>
       </c>
       <c r="AA83" s="6" t="n">
         <v>0</v>
@@ -6006,7 +6006,7 @@
         <v>0</v>
       </c>
       <c r="M84" s="6" t="n">
-        <v>0.00216535343279151</v>
+        <v>0.00216535343279152</v>
       </c>
       <c r="N84" s="6" t="n">
         <v>0</v>
@@ -6166,7 +6166,7 @@
         <v>0</v>
       </c>
       <c r="E89" s="1" t="n">
-        <v>0.000000000000000000230172103231791</v>
+        <v>0.000000000000000000072770526706567</v>
       </c>
       <c r="F89" s="1" t="n">
         <v>0</v>
@@ -6175,22 +6175,22 @@
         <v>0</v>
       </c>
       <c r="H89" s="1" t="n">
-        <v>0.000753992924168832</v>
+        <v>0.000753992924168837</v>
       </c>
       <c r="I89" s="1" t="n">
-        <v>0.0223774789351496</v>
+        <v>0.0223774789351495</v>
       </c>
       <c r="J89" s="1" t="n">
-        <v>0.00485670712315128</v>
+        <v>0.00485670712315105</v>
       </c>
       <c r="K89" s="1" t="n">
-        <v>0.000579647283232601</v>
+        <v>0.0005796472832326</v>
       </c>
       <c r="L89" s="1" t="n">
         <v>0</v>
       </c>
       <c r="M89" s="1" t="n">
-        <v>0.0034325274521146</v>
+        <v>0.00343252745211458</v>
       </c>
       <c r="N89" s="1" t="n">
         <v>0</v>
@@ -6205,7 +6205,7 @@
         <v>0.000000260965220344131</v>
       </c>
       <c r="R89" s="1" t="n">
-        <v>78.010810471011</v>
+        <v>78.0108104710106</v>
       </c>
       <c r="S89" s="1" t="n">
         <v>0</v>
@@ -6226,7 +6226,7 @@
         <v>0</v>
       </c>
       <c r="Y89" s="1" t="n">
-        <v>0.0000377592490531492</v>
+        <v>0.000037759249053149</v>
       </c>
       <c r="Z89" s="1" t="n">
         <v>0</v>
@@ -6246,7 +6246,7 @@
         <v>30</v>
       </c>
       <c r="B90" s="1" t="n">
-        <v>0.00250423005612496</v>
+        <v>0.00250423005612497</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>0</v>
@@ -6264,10 +6264,10 @@
         <v>0</v>
       </c>
       <c r="H90" s="1" t="n">
-        <v>0.00331027231610428</v>
+        <v>0.00331027231610433</v>
       </c>
       <c r="I90" s="1" t="n">
-        <v>0.0000791571234708902</v>
+        <v>0.0000791571234708918</v>
       </c>
       <c r="J90" s="1" t="n">
         <v>0</v>
@@ -6282,7 +6282,7 @@
         <v>0</v>
       </c>
       <c r="N90" s="1" t="n">
-        <v>0.000392246548936757</v>
+        <v>0.000392246548936754</v>
       </c>
       <c r="O90" s="1" t="n">
         <v>0</v>
@@ -6294,16 +6294,16 @@
         <v>0</v>
       </c>
       <c r="R90" s="1" t="n">
-        <v>26.2904528311585</v>
+        <v>26.2904528311589</v>
       </c>
       <c r="S90" s="1" t="n">
-        <v>0.000185976854428328</v>
+        <v>0.00018597685442833</v>
       </c>
       <c r="T90" s="1" t="n">
-        <v>0.0149970996640395</v>
+        <v>0.0149970996640393</v>
       </c>
       <c r="U90" s="1" t="n">
-        <v>0.352261790422132</v>
+        <v>0.352261790422136</v>
       </c>
       <c r="V90" s="1" t="n">
         <v>0</v>
@@ -6315,7 +6315,7 @@
         <v>0</v>
       </c>
       <c r="Y90" s="1" t="n">
-        <v>0.00759807742213925</v>
+        <v>0.00759807742213918</v>
       </c>
       <c r="Z90" s="1" t="n">
         <v>0</v>
@@ -6324,10 +6324,10 @@
         <v>0.00000666608625205579</v>
       </c>
       <c r="AB90" s="1" t="n">
-        <v>0.0000986853739616356</v>
+        <v>0.0000986853739616354</v>
       </c>
       <c r="AC90" s="1" t="n">
-        <v>0.00000350846644845042</v>
+        <v>0.00000350846644845039</v>
       </c>
     </row>
     <row r="91">
@@ -6347,7 +6347,7 @@
         <v>0</v>
       </c>
       <c r="F91" s="1" t="n">
-        <v>-0.00000000000000000000000249307932899137</v>
+        <v>-0.00000000000000000000000472872076711893</v>
       </c>
       <c r="G91" s="1" t="n">
         <v>0</v>
@@ -6380,7 +6380,7 @@
         <v>0</v>
       </c>
       <c r="Q91" s="1" t="n">
-        <v>0.000000170001616545434</v>
+        <v>0.000000170001616545435</v>
       </c>
       <c r="R91" s="1" t="n">
         <v>0</v>
@@ -6392,7 +6392,7 @@
         <v>0</v>
       </c>
       <c r="U91" s="1" t="n">
-        <v>0.00908445906200498</v>
+        <v>0.00908445906200507</v>
       </c>
       <c r="V91" s="1" t="n">
         <v>0</v>
@@ -7106,7 +7106,7 @@
         <v>0</v>
       </c>
       <c r="AJ6" s="7" t="n">
-        <v>0.000689849695048997</v>
+        <v>0.000689849695048991</v>
       </c>
       <c r="AK6" s="7" t="n">
         <v>0</v>
@@ -7118,7 +7118,7 @@
         <v>0</v>
       </c>
       <c r="AN6" s="7" t="n">
-        <v>0.00803046316801048</v>
+        <v>0.00803046316801043</v>
       </c>
       <c r="AO6" s="7" t="n">
         <v>0</v>
@@ -7133,7 +7133,7 @@
         <v>0</v>
       </c>
       <c r="AS6" s="7" t="n">
-        <v>0.000912547222807827</v>
+        <v>0.000912547222807832</v>
       </c>
       <c r="AT6" s="7" t="n">
         <v>0</v>
@@ -7887,7 +7887,7 @@
         <v>0</v>
       </c>
       <c r="AI14" s="7" t="n">
-        <v>0.00574284175091262</v>
+        <v>0.00574284175091277</v>
       </c>
       <c r="AJ14" s="7" t="n">
         <v>0</v>
@@ -7932,7 +7932,7 @@
         <v>0</v>
       </c>
       <c r="AZ14" s="7" t="n">
-        <v>0.72465121788954</v>
+        <v>0.724651217889545</v>
       </c>
       <c r="BA14" s="7" t="n">
         <v>0</v>
@@ -8211,7 +8211,7 @@
         <v>0</v>
       </c>
       <c r="AS17" s="7" t="n">
-        <v>0.00124523293801619</v>
+        <v>0.00124523293801618</v>
       </c>
       <c r="AT17" s="7" t="n">
         <v>0</v>
@@ -8661,7 +8661,7 @@
         <v>0</v>
       </c>
       <c r="AJ25" s="7" t="n">
-        <v>0.00533530326728261</v>
+        <v>0.00533530326728257</v>
       </c>
       <c r="AK25" s="7" t="n">
         <v>0</v>
@@ -8705,7 +8705,7 @@
         <v>5</v>
       </c>
       <c r="AG26" s="7" t="n">
-        <v>-0.0000000000000000164261668334763</v>
+        <v>0.00000000000000000521647247225336</v>
       </c>
       <c r="AH26" s="7" t="n">
         <v>0</v>
@@ -8767,10 +8767,10 @@
         <v>0</v>
       </c>
       <c r="AJ27" s="7" t="n">
-        <v>0.00785182196196129</v>
+        <v>0.00785182196196112</v>
       </c>
       <c r="AK27" s="7" t="n">
-        <v>-0.0000000000000000237499455684004</v>
+        <v>0.00000000000000000754229142629843</v>
       </c>
       <c r="AL27" s="7" t="n">
         <v>0</v>
@@ -8844,7 +8844,7 @@
         <v>0</v>
       </c>
       <c r="AR28" s="7" t="n">
-        <v>0.000083906465249669</v>
+        <v>0.0000839064652496701</v>
       </c>
       <c r="AS28" s="7" t="n">
         <v>0.0265576675615998</v>
@@ -8991,7 +8991,7 @@
         <v>0</v>
       </c>
       <c r="AN31" s="7" t="n">
-        <v>0.000299428166183029</v>
+        <v>0.000299428166183027</v>
       </c>
       <c r="AO31" s="7" t="n">
         <v>0</v>
@@ -9044,10 +9044,10 @@
         <v>0</v>
       </c>
       <c r="AN32" s="7" t="n">
-        <v>0.000575922626328547</v>
+        <v>0.000575922626328543</v>
       </c>
       <c r="AO32" s="7" t="n">
-        <v>0.000192133559819273</v>
+        <v>0.000192133559819271</v>
       </c>
       <c r="AP32" s="7" t="n">
         <v>0</v>
@@ -9145,7 +9145,7 @@
         <v>0</v>
       </c>
       <c r="AM34" s="7" t="n">
-        <v>0.00102952813067239</v>
+        <v>0.00102952813067237</v>
       </c>
       <c r="AN34" s="7" t="n">
         <v>0</v>
@@ -9154,7 +9154,7 @@
         <v>0</v>
       </c>
       <c r="AP34" s="7" t="n">
-        <v>27.3420709432359</v>
+        <v>27.3420709432362</v>
       </c>
       <c r="AQ34" s="7" t="n">
         <v>0</v>
@@ -9207,10 +9207,10 @@
         <v>0</v>
       </c>
       <c r="AR35" s="7" t="n">
-        <v>0.000193415731217961</v>
+        <v>0.00019341573121796</v>
       </c>
       <c r="AS35" s="7" t="n">
-        <v>0.000193415731217961</v>
+        <v>0.00019341573121796</v>
       </c>
       <c r="AT35" s="7" t="n">
         <v>0</v>
@@ -9245,13 +9245,13 @@
         <v>0</v>
       </c>
       <c r="AO36" s="7" t="n">
-        <v>0.00734600764041628</v>
+        <v>0.00734600764041616</v>
       </c>
       <c r="AP36" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AQ36" s="7" t="n">
-        <v>0.0220197451047994</v>
+        <v>0.0220197451047991</v>
       </c>
       <c r="AR36" s="7" t="n">
         <v>0</v>
@@ -9277,19 +9277,19 @@
         <v>0.00218213182139153</v>
       </c>
       <c r="AJ37" s="7" t="n">
-        <v>0.366301487805043</v>
+        <v>0.366301487805041</v>
       </c>
       <c r="AK37" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AL37" s="7" t="n">
-        <v>0.000000000000000045226592442112</v>
+        <v>0.0000000000000000749668715899822</v>
       </c>
       <c r="AM37" s="7" t="n">
         <v>0</v>
       </c>
       <c r="AN37" s="7" t="n">
-        <v>0.382064617197644</v>
+        <v>0.382064617197642</v>
       </c>
       <c r="AO37" s="7" t="n">
         <v>0</v>
@@ -9354,7 +9354,7 @@
         <v>0</v>
       </c>
       <c r="AT38" s="7" t="n">
-        <v>0.00214498176865486</v>
+        <v>0.00214498176865492</v>
       </c>
     </row>
     <row r="39">
@@ -9365,7 +9365,7 @@
         <v>0</v>
       </c>
       <c r="AH39" s="7" t="n">
-        <v>0.00000000000000000147529976698872</v>
+        <v>-0.00000000000000000147265996373125</v>
       </c>
       <c r="AI39" s="7" t="n">
         <v>0</v>
@@ -9383,10 +9383,10 @@
         <v>0</v>
       </c>
       <c r="AN39" s="7" t="n">
-        <v>0.000601951329799318</v>
+        <v>0.000601951329799324</v>
       </c>
       <c r="AO39" s="7" t="n">
-        <v>0.0155838602661988</v>
+        <v>0.0155838602661987</v>
       </c>
       <c r="AP39" s="7" t="n">
         <v>0</v>
@@ -9477,10 +9477,10 @@
         <v>0</v>
       </c>
       <c r="AN41" s="7" t="n">
-        <v>0.00000978759382848156</v>
+        <v>0.00000978759382848157</v>
       </c>
       <c r="AO41" s="7" t="n">
-        <v>0.00000326523938869963</v>
+        <v>0.00000326523938869961</v>
       </c>
       <c r="AP41" s="7" t="n">
         <v>0</v>
@@ -9527,7 +9527,7 @@
         <v>0</v>
       </c>
       <c r="AO42" s="7" t="n">
-        <v>0.0000454541155136077</v>
+        <v>0.0000454541155136074</v>
       </c>
       <c r="AP42" s="7" t="n">
         <v>0</v>
@@ -9571,10 +9571,10 @@
         <v>0</v>
       </c>
       <c r="AN43" s="7" t="n">
-        <v>0.00000515136517288503</v>
+        <v>0.000005151365172885</v>
       </c>
       <c r="AO43" s="7" t="n">
-        <v>0.00000171854704668402</v>
+        <v>0.00000171854704668399</v>
       </c>
       <c r="AP43" s="7" t="n">
         <v>0</v>
@@ -9665,7 +9665,7 @@
         <v>0</v>
       </c>
       <c r="AJ48" s="6" t="n">
-        <v>0.00533530326728261</v>
+        <v>0.00533530326728257</v>
       </c>
       <c r="AK48" s="6" t="n">
         <v>0</v>
@@ -9709,7 +9709,7 @@
         <v>5</v>
       </c>
       <c r="AG49" s="6" t="n">
-        <v>-0.0000000000000000164261668334763</v>
+        <v>0.00000000000000000521647247225336</v>
       </c>
       <c r="AH49" s="6" t="n">
         <v>0</v>
@@ -9771,10 +9771,10 @@
         <v>0</v>
       </c>
       <c r="AJ50" s="6" t="n">
-        <v>0.00785182196196129</v>
+        <v>0.00785182196196112</v>
       </c>
       <c r="AK50" s="6" t="n">
-        <v>-0.0000000000000000237499455684004</v>
+        <v>0.00000000000000000754229142629843</v>
       </c>
       <c r="AL50" s="6" t="n">
         <v>0</v>
@@ -9848,7 +9848,7 @@
         <v>0</v>
       </c>
       <c r="AR51" s="6" t="n">
-        <v>0.000083906465249669</v>
+        <v>0.0000839064652496701</v>
       </c>
       <c r="AS51" s="6" t="n">
         <v>0.0265576675615998</v>
@@ -9877,7 +9877,7 @@
         <v>0</v>
       </c>
       <c r="AJ52" s="6" t="n">
-        <v>0.000689849695048997</v>
+        <v>0.000689849695048991</v>
       </c>
       <c r="AK52" s="6" t="n">
         <v>0</v>
@@ -9889,7 +9889,7 @@
         <v>0</v>
       </c>
       <c r="AN52" s="6" t="n">
-        <v>0.00803046316801048</v>
+        <v>0.00803046316801043</v>
       </c>
       <c r="AO52" s="6" t="n">
         <v>0</v>
@@ -9904,7 +9904,7 @@
         <v>0</v>
       </c>
       <c r="AS52" s="6" t="n">
-        <v>0.000912547222807827</v>
+        <v>0.000912547222807832</v>
       </c>
       <c r="AT52" s="6" t="n">
         <v>0</v>
@@ -9995,7 +9995,7 @@
         <v>0</v>
       </c>
       <c r="AN54" s="6" t="n">
-        <v>0.000299428166183029</v>
+        <v>0.000299428166183027</v>
       </c>
       <c r="AO54" s="6" t="n">
         <v>0</v>
@@ -10048,10 +10048,10 @@
         <v>0</v>
       </c>
       <c r="AN55" s="6" t="n">
-        <v>0.000575922626328547</v>
+        <v>0.000575922626328543</v>
       </c>
       <c r="AO55" s="6" t="n">
-        <v>0.000192133559819273</v>
+        <v>0.000192133559819271</v>
       </c>
       <c r="AP55" s="6" t="n">
         <v>0</v>
@@ -10151,7 +10151,7 @@
         <v>0</v>
       </c>
       <c r="AM57" s="6" t="n">
-        <v>0.00102952813067239</v>
+        <v>0.00102952813067237</v>
       </c>
       <c r="AN57" s="6" t="n">
         <v>0</v>
@@ -10160,7 +10160,7 @@
         <v>0</v>
       </c>
       <c r="AP57" s="6" t="n">
-        <v>27.3420709432359</v>
+        <v>27.3420709432362</v>
       </c>
       <c r="AQ57" s="6" t="n">
         <v>0</v>
@@ -10219,10 +10219,10 @@
         <v>0</v>
       </c>
       <c r="AR58" s="6" t="n">
-        <v>0.000193415731217961</v>
+        <v>0.00019341573121796</v>
       </c>
       <c r="AS58" s="6" t="n">
-        <v>0.000193415731217961</v>
+        <v>0.00019341573121796</v>
       </c>
       <c r="AT58" s="6" t="n">
         <v>0</v>
@@ -10263,13 +10263,13 @@
         <v>0</v>
       </c>
       <c r="AO59" s="6" t="n">
-        <v>0.00734600764041628</v>
+        <v>0.00734600764041616</v>
       </c>
       <c r="AP59" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AQ59" s="6" t="n">
-        <v>0.0220197451047994</v>
+        <v>0.0220197451047991</v>
       </c>
       <c r="AR59" s="6" t="n">
         <v>0</v>
@@ -10298,22 +10298,22 @@
         <v>0</v>
       </c>
       <c r="AI60" s="6" t="n">
-        <v>0.00792497357230415</v>
+        <v>0.0079249735723043</v>
       </c>
       <c r="AJ60" s="6" t="n">
-        <v>0.366301487805043</v>
+        <v>0.366301487805041</v>
       </c>
       <c r="AK60" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AL60" s="6" t="n">
-        <v>0.000000000000000045226592442112</v>
+        <v>0.0000000000000000749668715899822</v>
       </c>
       <c r="AM60" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AN60" s="6" t="n">
-        <v>0.382064617197644</v>
+        <v>0.382064617197642</v>
       </c>
       <c r="AO60" s="6" t="n">
         <v>0</v>
@@ -10384,7 +10384,7 @@
         <v>0</v>
       </c>
       <c r="AT61" s="6" t="n">
-        <v>0.00214498176865486</v>
+        <v>0.00214498176865492</v>
       </c>
       <c r="AW61" s="4" t="s">
         <v>21</v>
@@ -10401,7 +10401,7 @@
         <v>0</v>
       </c>
       <c r="AH62" s="6" t="n">
-        <v>0.00000000000000000147529976698872</v>
+        <v>-0.00000000000000000147265996373125</v>
       </c>
       <c r="AI62" s="6" t="n">
         <v>0</v>
@@ -10419,10 +10419,10 @@
         <v>0</v>
       </c>
       <c r="AN62" s="6" t="n">
-        <v>0.000601951329799318</v>
+        <v>0.000601951329799324</v>
       </c>
       <c r="AO62" s="6" t="n">
-        <v>0.0155838602661988</v>
+        <v>0.0155838602661987</v>
       </c>
       <c r="AP62" s="6" t="n">
         <v>0</v>
@@ -10487,7 +10487,7 @@
         <v>0</v>
       </c>
       <c r="AS63" s="6" t="n">
-        <v>0.00124523293801619</v>
+        <v>0.00124523293801618</v>
       </c>
       <c r="AT63" s="6" t="n">
         <v>0</v>
@@ -10525,10 +10525,10 @@
         <v>0</v>
       </c>
       <c r="AN64" s="6" t="n">
-        <v>0.00000978759382848156</v>
+        <v>0.00000978759382848157</v>
       </c>
       <c r="AO64" s="6" t="n">
-        <v>0.00000326523938869963</v>
+        <v>0.00000326523938869961</v>
       </c>
       <c r="AP64" s="6" t="n">
         <v>0</v>
@@ -10581,7 +10581,7 @@
         <v>0</v>
       </c>
       <c r="AO65" s="6" t="n">
-        <v>0.0000454541155136077</v>
+        <v>0.0000454541155136074</v>
       </c>
       <c r="AP65" s="6" t="n">
         <v>0</v>
@@ -10631,10 +10631,10 @@
         <v>0</v>
       </c>
       <c r="AN66" s="6" t="n">
-        <v>0.00000515136517288503</v>
+        <v>0.000005151365172885</v>
       </c>
       <c r="AO66" s="6" t="n">
-        <v>0.00000171854704668402</v>
+        <v>0.00000171854704668399</v>
       </c>
       <c r="AP66" s="6" t="n">
         <v>0</v>
@@ -10768,7 +10768,7 @@
         <v>0</v>
       </c>
       <c r="D71" s="6" t="n">
-        <v>-0.00000000000000000650788310863421</v>
+        <v>0.00000000000000000206671425129124</v>
       </c>
       <c r="E71" s="6" t="n">
         <v>0</v>
@@ -10860,7 +10860,7 @@
         <v>0</v>
       </c>
       <c r="E72" s="6" t="n">
-        <v>0.000000000000000000213597011110172</v>
+        <v>-0.000000000000000000213214814828217</v>
       </c>
       <c r="F72" s="6" t="n">
         <v>0</v>
@@ -11000,7 +11000,7 @@
         <v>0</v>
       </c>
       <c r="V73" s="6" t="n">
-        <v>0.00158573469356971</v>
+        <v>0.00158573469356977</v>
       </c>
       <c r="W73" s="6" t="n">
         <v>0</v>
@@ -11029,7 +11029,7 @@
         <v>37</v>
       </c>
       <c r="B74" s="6" t="n">
-        <v>0.00268081967118607</v>
+        <v>0.00268081967118606</v>
       </c>
       <c r="C74" s="6" t="n">
         <v>0</v>
@@ -11047,7 +11047,7 @@
         <v>0</v>
       </c>
       <c r="H74" s="6" t="n">
-        <v>0.00354370123475279</v>
+        <v>0.00354370123475275</v>
       </c>
       <c r="I74" s="6" t="n">
         <v>0</v>
@@ -11130,7 +11130,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="6" t="n">
-        <v>-0.0000000000000000164261644853625</v>
+        <v>0.00000000000000000521647172656076</v>
       </c>
       <c r="G75" s="6" t="n">
         <v>0</v>
@@ -11237,7 +11237,7 @@
         <v>0</v>
       </c>
       <c r="L76" s="6" t="n">
-        <v>0.0000000000000000119357521981296</v>
+        <v>0.0000000000000000197845107060036</v>
       </c>
       <c r="M76" s="6" t="n">
         <v>0</v>
@@ -11356,7 +11356,7 @@
         <v>0</v>
       </c>
       <c r="V77" s="6" t="n">
-        <v>0.000559247075085147</v>
+        <v>0.000559247075085158</v>
       </c>
       <c r="W77" s="6" t="n">
         <v>0</v>
@@ -11510,7 +11510,7 @@
         <v>0</v>
       </c>
       <c r="N79" s="6" t="n">
-        <v>0.00038402809307391</v>
+        <v>0.000384028093073907</v>
       </c>
       <c r="O79" s="6" t="n">
         <v>0</v>
@@ -11528,7 +11528,7 @@
         <v>0</v>
       </c>
       <c r="T79" s="6" t="n">
-        <v>0.0146828763726078</v>
+        <v>0.0146828763726077</v>
       </c>
       <c r="U79" s="6" t="n">
         <v>0</v>
@@ -11543,19 +11543,19 @@
         <v>0</v>
       </c>
       <c r="Y79" s="6" t="n">
-        <v>0.00807284647222644</v>
+        <v>0.00807284647222639</v>
       </c>
       <c r="Z79" s="6" t="n">
         <v>0</v>
       </c>
       <c r="AA79" s="6" t="n">
-        <v>0.0000065264166085906</v>
+        <v>0.00000652641660859059</v>
       </c>
       <c r="AB79" s="6" t="n">
-        <v>0.0000227270577568039</v>
+        <v>0.0000227270577568037</v>
       </c>
       <c r="AC79" s="6" t="n">
-        <v>0.00000343495610978452</v>
+        <v>0.0000034349561097845</v>
       </c>
     </row>
     <row r="80">
@@ -11611,7 +11611,7 @@
         <v>0</v>
       </c>
       <c r="R80" s="6" t="n">
-        <v>27.3420709432359</v>
+        <v>27.3420709432362</v>
       </c>
       <c r="S80" s="6" t="n">
         <v>0</v>
@@ -11676,7 +11676,7 @@
         <v>0</v>
       </c>
       <c r="J81" s="6" t="n">
-        <v>0.0072665158845838</v>
+        <v>0.00726651588458383</v>
       </c>
       <c r="K81" s="6" t="n">
         <v>0</v>
@@ -11762,7 +11762,7 @@
         <v>0</v>
       </c>
       <c r="I82" s="6" t="n">
-        <v>0.000083906465249669</v>
+        <v>0.0000839064652496701</v>
       </c>
       <c r="J82" s="6" t="n">
         <v>0</v>
@@ -11792,7 +11792,7 @@
         <v>0</v>
       </c>
       <c r="S82" s="6" t="n">
-        <v>0.000193415731217961</v>
+        <v>0.00019341573121796</v>
       </c>
       <c r="T82" s="6" t="n">
         <v>0</v>
@@ -11863,7 +11863,7 @@
         <v>0</v>
       </c>
       <c r="M83" s="6" t="n">
-        <v>0.00595909702035804</v>
+        <v>0.00595909702035798</v>
       </c>
       <c r="N83" s="6" t="n">
         <v>0</v>
@@ -11902,7 +11902,7 @@
         <v>0</v>
       </c>
       <c r="Z83" s="6" t="n">
-        <v>0.00124523293801619</v>
+        <v>0.00124523293801618</v>
       </c>
       <c r="AA83" s="6" t="n">
         <v>0</v>
@@ -11952,7 +11952,7 @@
         <v>0</v>
       </c>
       <c r="M84" s="6" t="n">
-        <v>0.002295274638305</v>
+        <v>0.00229527463830508</v>
       </c>
       <c r="N84" s="6" t="n">
         <v>0</v>
@@ -12112,7 +12112,7 @@
         <v>0</v>
       </c>
       <c r="E89" s="1" t="n">
-        <v>-0.000000000000000000213597011110172</v>
+        <v>0.000000000000000000213214814828217</v>
       </c>
       <c r="F89" s="1" t="n">
         <v>0</v>
@@ -12121,22 +12121,22 @@
         <v>0</v>
       </c>
       <c r="H89" s="1" t="n">
-        <v>0.000799232420313688</v>
+        <v>0.00079923242031368</v>
       </c>
       <c r="I89" s="1" t="n">
         <v>0.0237201034640655</v>
       </c>
       <c r="J89" s="1" t="n">
-        <v>0.00485670708499603</v>
+        <v>0.00485670708499579</v>
       </c>
       <c r="K89" s="1" t="n">
-        <v>0.000614426120226556</v>
+        <v>0.000614426120226557</v>
       </c>
       <c r="L89" s="1" t="n">
         <v>0</v>
       </c>
       <c r="M89" s="1" t="n">
-        <v>0.00363847909852179</v>
+        <v>0.00363847909852177</v>
       </c>
       <c r="N89" s="1" t="n">
         <v>0</v>
@@ -12151,7 +12151,7 @@
         <v>0.000000271403829157896</v>
       </c>
       <c r="R89" s="1" t="n">
-        <v>81.1312428863831</v>
+        <v>81.131242886383</v>
       </c>
       <c r="S89" s="1" t="n">
         <v>0</v>
@@ -12172,7 +12172,7 @@
         <v>0</v>
       </c>
       <c r="Y89" s="1" t="n">
-        <v>0.0000401186515452501</v>
+        <v>0.0000401186515452477</v>
       </c>
       <c r="Z89" s="1" t="n">
         <v>0</v>
@@ -12192,7 +12192,7 @@
         <v>30</v>
       </c>
       <c r="B90" s="1" t="n">
-        <v>0.00265448359609654</v>
+        <v>0.00265448359609652</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>0</v>
@@ -12210,10 +12210,10 @@
         <v>0</v>
       </c>
       <c r="H90" s="1" t="n">
-        <v>0.00350888830689479</v>
+        <v>0.00350888830689469</v>
       </c>
       <c r="I90" s="1" t="n">
-        <v>0.0000839064652496689</v>
+        <v>0.0000839064652496703</v>
       </c>
       <c r="J90" s="1" t="n">
         <v>0</v>
@@ -12228,7 +12228,7 @@
         <v>0</v>
       </c>
       <c r="N90" s="1" t="n">
-        <v>0.00038402809307391</v>
+        <v>0.000384028093073906</v>
       </c>
       <c r="O90" s="1" t="n">
         <v>0</v>
@@ -12240,16 +12240,16 @@
         <v>0</v>
       </c>
       <c r="R90" s="1" t="n">
-        <v>27.3420709432359</v>
+        <v>27.3420709432361</v>
       </c>
       <c r="S90" s="1" t="n">
-        <v>0.000193415731217961</v>
+        <v>0.00019341573121796</v>
       </c>
       <c r="T90" s="1" t="n">
-        <v>0.0146828763726078</v>
+        <v>0.0146828763726076</v>
       </c>
       <c r="U90" s="1" t="n">
-        <v>0.373397460796425</v>
+        <v>0.373397460796421</v>
       </c>
       <c r="V90" s="1" t="n">
         <v>0</v>
@@ -12261,19 +12261,19 @@
         <v>0</v>
       </c>
       <c r="Y90" s="1" t="n">
-        <v>0.00807284647222644</v>
+        <v>0.0080728464722264</v>
       </c>
       <c r="Z90" s="1" t="n">
         <v>0</v>
       </c>
       <c r="AA90" s="1" t="n">
-        <v>0.0000065264166085906</v>
+        <v>0.00000652641660859059</v>
       </c>
       <c r="AB90" s="1" t="n">
-        <v>0.0000227270577568038</v>
+        <v>0.0000227270577568037</v>
       </c>
       <c r="AC90" s="1" t="n">
-        <v>0.00000343495610978452</v>
+        <v>0.0000034349561097845</v>
       </c>
     </row>
     <row r="91">
@@ -12293,7 +12293,7 @@
         <v>0</v>
       </c>
       <c r="F91" s="1" t="n">
-        <v>-0.0000000000000000000000023481138271128</v>
+        <v>0.000000000000000000000000745692602231639</v>
       </c>
       <c r="G91" s="1" t="n">
         <v>0</v>
@@ -12302,13 +12302,13 @@
         <v>0</v>
       </c>
       <c r="I91" s="1" t="n">
-        <v>0.00257058898083077</v>
+        <v>0.00257058898083076</v>
       </c>
       <c r="J91" s="1" t="n">
         <v>0</v>
       </c>
       <c r="K91" s="1" t="n">
-        <v>0.000446329114089545</v>
+        <v>0.000446329114089547</v>
       </c>
       <c r="L91" s="1" t="n">
         <v>0</v>
@@ -12338,10 +12338,10 @@
         <v>0</v>
       </c>
       <c r="U91" s="1" t="n">
-        <v>0.00962952565021816</v>
+        <v>0.00962952565021775</v>
       </c>
       <c r="V91" s="1" t="n">
-        <v>-0.000000000000000000433680868994202</v>
+        <v>0</v>
       </c>
       <c r="W91" s="1" t="n">
         <v>0</v>
@@ -12391,7 +12391,7 @@
         <v>0</v>
       </c>
       <c r="I92" s="1" t="n">
-        <v>0.000183068651453823</v>
+        <v>0.000183068651453825</v>
       </c>
       <c r="J92" s="1" t="n">
         <v>0</v>

</xml_diff>